<commit_message>
chore: add throughput test results
</commit_message>
<xml_diff>
--- a/load-testing/workbench/results.xlsx
+++ b/load-testing/workbench/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Server 3.5.0 (AWS)" sheetId="1" state="visible" r:id="rId2"/>
@@ -253,16 +253,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N31" activeCellId="0" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,24 +831,6 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -865,16 +847,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,22 +902,40 @@
       <c r="B2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="e">
+      <c r="C2" s="4" t="n">
         <f aca="false">AVERAGE(F2:L2)</f>
-        <v>#DIV/0!</v>
+        <v>1135.71428571429</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">MIN(F2:L2)</f>
-        <v>0</v>
+        <v>1130</v>
       </c>
       <c r="E2" s="1" t="n">
         <f aca="false">MAX(F2:L2)</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="5" t="e">
-        <f aca="false">(C2-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>1141</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1130</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1141</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1134</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1132</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>1139</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1140</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1134</v>
+      </c>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -944,21 +944,42 @@
       <c r="B3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="e">
+      <c r="C3" s="4" t="n">
         <f aca="false">AVERAGE(F3:L3)</f>
-        <v>#DIV/0!</v>
+        <v>1139.85714285714</v>
       </c>
       <c r="D3" s="1" t="n">
         <f aca="false">MIN(F3:L3)</f>
-        <v>0</v>
+        <v>1130</v>
       </c>
       <c r="E3" s="1" t="n">
         <f aca="false">MAX(F3:L3)</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="5" t="e">
-        <f aca="false">(C3-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>1148</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1130</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1148</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1141</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1139</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1143</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>1141</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>1137</v>
+      </c>
+      <c r="N3" s="5" t="n">
+        <f aca="false">(C3-$C$2)/$C$2</f>
+        <v>0.00364779874213834</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,21 +989,42 @@
       <c r="B4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="e">
+      <c r="C4" s="4" t="n">
         <f aca="false">AVERAGE(F4:L4)</f>
-        <v>#DIV/0!</v>
+        <v>1011.57142857143</v>
       </c>
       <c r="D4" s="1" t="n">
         <f aca="false">MIN(F4:L4)</f>
-        <v>0</v>
+        <v>1006</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="false">MAX(F4:L4)</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="5" t="e">
-        <f aca="false">(C4-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>1022</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1022</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1006</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1014</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1011</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1014</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1008</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1006</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <f aca="false">(C4-$C$2)/$C$2</f>
+        <v>-0.109308176100629</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,21 +1034,42 @@
       <c r="B5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="e">
+      <c r="C5" s="4" t="n">
         <f aca="false">AVERAGE(F5:L5)</f>
-        <v>#DIV/0!</v>
+        <v>2060</v>
       </c>
       <c r="D5" s="1" t="n">
         <f aca="false">MIN(F5:L5)</f>
-        <v>0</v>
+        <v>2025</v>
       </c>
       <c r="E5" s="1" t="n">
         <f aca="false">MAX(F5:L5)</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="5" t="e">
-        <f aca="false">(C5-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>2091</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>2025</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>2058</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>2085</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>2078</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>2058</v>
+      </c>
+      <c r="N5" s="5" t="n">
+        <f aca="false">(C5-$C$2)/$C$2</f>
+        <v>0.813836477987421</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,21 +1079,42 @@
       <c r="B6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="e">
+      <c r="C6" s="4" t="n">
         <f aca="false">AVERAGE(F6:L6)</f>
-        <v>#DIV/0!</v>
+        <v>2092.71428571429</v>
       </c>
       <c r="D6" s="1" t="n">
         <f aca="false">MIN(F6:L6)</f>
-        <v>0</v>
+        <v>2078</v>
       </c>
       <c r="E6" s="1" t="n">
         <f aca="false">MAX(F6:L6)</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="5" t="e">
-        <f aca="false">(C6-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>2111</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>2096</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>2111</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>2087</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>2078</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>2098</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>2093</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>2086</v>
+      </c>
+      <c r="N6" s="5" t="n">
+        <f aca="false">(C6-$C$2)/$C$2</f>
+        <v>0.842641509433962</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,21 +1124,42 @@
       <c r="B7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="4" t="e">
+      <c r="C7" s="4" t="n">
         <f aca="false">AVERAGE(F7:L7)</f>
-        <v>#DIV/0!</v>
+        <v>1869.42857142857</v>
       </c>
       <c r="D7" s="1" t="n">
         <f aca="false">MIN(F7:L7)</f>
-        <v>0</v>
+        <v>1852</v>
       </c>
       <c r="E7" s="1" t="n">
         <f aca="false">MAX(F7:L7)</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="5" t="e">
-        <f aca="false">(C7-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>1882</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1877</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1882</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1863</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1868</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1873</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>1852</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>1871</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <f aca="false">(C7-$C$2)/$C$2</f>
+        <v>0.646037735849056</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,21 +1169,42 @@
       <c r="B8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="e">
+      <c r="C8" s="4" t="n">
         <f aca="false">AVERAGE(F8:L8)</f>
-        <v>#DIV/0!</v>
+        <v>2481.42857142857</v>
       </c>
       <c r="D8" s="1" t="n">
         <f aca="false">MIN(F8:L8)</f>
-        <v>0</v>
+        <v>2469</v>
       </c>
       <c r="E8" s="1" t="n">
         <f aca="false">MAX(F8:L8)</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="5" t="e">
-        <f aca="false">(C8-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>2501</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2478</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>2501</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>2470</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>2469</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>2492</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>2485</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>2475</v>
+      </c>
+      <c r="N8" s="5" t="n">
+        <f aca="false">(C8-$C$2)/$C$2</f>
+        <v>1.18490566037736</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1088,21 +1214,42 @@
       <c r="B9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="e">
+      <c r="C9" s="4" t="n">
         <f aca="false">AVERAGE(F9:L9)</f>
-        <v>#DIV/0!</v>
+        <v>2505.71428571429</v>
       </c>
       <c r="D9" s="1" t="n">
         <f aca="false">MIN(F9:L9)</f>
-        <v>0</v>
+        <v>2484</v>
       </c>
       <c r="E9" s="1" t="n">
         <f aca="false">MAX(F9:L9)</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="5" t="e">
-        <f aca="false">(C9-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>2522</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>2506</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>2522</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>2511</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>2503</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>2484</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>2508</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>2506</v>
+      </c>
+      <c r="N9" s="5" t="n">
+        <f aca="false">(C9-$C$2)/$C$2</f>
+        <v>1.2062893081761</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,21 +1259,42 @@
       <c r="B10" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4" t="e">
+      <c r="C10" s="4" t="n">
         <f aca="false">AVERAGE(F10:L10)</f>
-        <v>#DIV/0!</v>
+        <v>2184</v>
       </c>
       <c r="D10" s="1" t="n">
         <f aca="false">MIN(F10:L10)</f>
-        <v>0</v>
+        <v>2149</v>
       </c>
       <c r="E10" s="1" t="n">
         <f aca="false">MAX(F10:L10)</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="5" t="e">
-        <f aca="false">(C10-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>2229</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>2149</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>2227</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>2152</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>2229</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>2153</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>2182</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>2196</v>
+      </c>
+      <c r="N10" s="5" t="n">
+        <f aca="false">(C10-$C$2)/$C$2</f>
+        <v>0.923018867924528</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,21 +1304,42 @@
       <c r="B11" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="4" t="e">
+      <c r="C11" s="4" t="n">
         <f aca="false">AVERAGE(F11:L11)</f>
-        <v>#DIV/0!</v>
+        <v>1297</v>
       </c>
       <c r="D11" s="1" t="n">
         <f aca="false">MIN(F11:L11)</f>
-        <v>0</v>
+        <v>1293</v>
       </c>
       <c r="E11" s="1" t="n">
         <f aca="false">MAX(F11:L11)</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="5" t="e">
-        <f aca="false">(C11-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>1300</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>1297</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1296</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1297</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>1297</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>1293</v>
+      </c>
+      <c r="N11" s="5" t="n">
+        <f aca="false">(C11-$C$2)/$C$2</f>
+        <v>0.142012578616352</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,21 +1349,42 @@
       <c r="B12" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4" t="e">
+      <c r="C12" s="4" t="n">
         <f aca="false">AVERAGE(F12:L12)</f>
-        <v>#DIV/0!</v>
+        <v>1241.57142857143</v>
       </c>
       <c r="D12" s="1" t="n">
         <f aca="false">MIN(F12:L12)</f>
-        <v>0</v>
+        <v>1236</v>
       </c>
       <c r="E12" s="1" t="n">
         <f aca="false">MAX(F12:L12)</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="5" t="e">
-        <f aca="false">(C12-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>1246</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1244</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1236</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1242</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1244</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1246</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>1241</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>1238</v>
+      </c>
+      <c r="N12" s="5" t="n">
+        <f aca="false">(C12-$C$2)/$C$2</f>
+        <v>0.0932075471698114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1184,21 +1394,42 @@
       <c r="B13" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4" t="e">
+      <c r="C13" s="4" t="n">
         <f aca="false">AVERAGE(F13:L13)</f>
-        <v>#DIV/0!</v>
+        <v>1094.14285714286</v>
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">MIN(F13:L13)</f>
-        <v>0</v>
+        <v>1064</v>
       </c>
       <c r="E13" s="1" t="n">
         <f aca="false">MAX(F13:L13)</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="5" t="e">
-        <f aca="false">(C13-#REF!)/#REF!</f>
-        <v>#DIV/0!</v>
+        <v>1120</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1116</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>1079</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>1094</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>1120</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1103</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>1064</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>1083</v>
+      </c>
+      <c r="N13" s="5" t="n">
+        <f aca="false">(C13-$C$2)/$C$2</f>
+        <v>-0.0366037735849057</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,22 +1674,6 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1477,18 +1692,18 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1497,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>30</v>
       </c>
@@ -1509,7 +1724,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>31</v>
       </c>
@@ -1521,7 +1736,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>32</v>
       </c>
@@ -1533,7 +1748,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>30</v>
       </c>
@@ -1545,7 +1760,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>31</v>
       </c>
@@ -1557,7 +1772,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>32</v>
       </c>
@@ -1569,7 +1784,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>30</v>
       </c>
@@ -1581,7 +1796,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>31</v>
       </c>
@@ -1593,7 +1808,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>32</v>
       </c>
@@ -1605,7 +1820,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>30</v>
       </c>
@@ -1617,7 +1832,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>31</v>
       </c>
@@ -1626,10 +1841,10 @@
       </c>
       <c r="C12" s="6" t="e">
         <f aca="false">('Server 3.5.0 (Mac M2)'!C12-'Server 3.5.0 (AWS)'!C15)/'Server 3.5.0 (AWS)'!C15</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>32</v>
       </c>
@@ -1641,7 +1856,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1649,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>19</v>
       </c>
@@ -1658,7 +1873,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>20</v>
       </c>
@@ -1667,7 +1882,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>21</v>
       </c>
@@ -1676,7 +1891,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>22</v>
       </c>
@@ -1685,7 +1900,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>23</v>
       </c>
@@ -1694,7 +1909,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>24</v>
       </c>
@@ -1703,7 +1918,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +1927,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>26</v>
       </c>
@@ -1721,7 +1936,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>27</v>
       </c>
@@ -1730,7 +1945,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>28</v>
       </c>

</xml_diff>